<commit_message>
Fix df_index, put labels in barplots
- 27.ORK1 has an NA value for ecological tilstand
- Put labels at the end of the bars in the barplots (ver2 and ver3 of ecological plots)
- Changed landmass color to navajo white
</commit_message>
<xml_diff>
--- a/Data_input/2019/KartOgFigurgrunnlag_TilDag.xlsx
+++ b/Data_input/2019/KartOgFigurgrunnlag_TilDag.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Prosjekter\Ferskvann\16384 Elveovervåkingsprogrammet\2018\Opsjon 3, biologi\Rapportering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B58E191-9BDF-42F2-BAD5-A2BD87D212C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C23D0AE-316C-4683-B611-C7F8F9E3EAA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{17B4FA25-9B82-482B-8BDB-C8E0043C0820}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{17B4FA25-9B82-482B-8BDB-C8E0043C0820}"/>
   </bookViews>
   <sheets>
     <sheet name="Figurgrunnlag" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="171">
   <si>
     <t>Vann- forekomst, kortnavn</t>
   </si>
@@ -554,7 +554,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,6 +645,26 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -708,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -744,12 +764,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -850,6 +885,30 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1168,16 +1227,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D75DE1-C95B-4F6D-BDBB-A1FD806C4458}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="18" customWidth="1"/>
     <col min="3" max="3" width="14" style="18" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="36" x14ac:dyDescent="0.3">
@@ -1226,42 +1285,42 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14">
-        <v>0.88210955282564507</v>
-      </c>
-      <c r="C4" s="19">
-        <v>0.56226670149326563</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0.56226670149326563</v>
+      <c r="B4" s="38">
+        <v>0.75660088604365472</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1.0013873473917871</v>
+      </c>
+      <c r="D4" s="38">
+        <v>0.75660088604365472</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.90781729220445795</v>
-      </c>
-      <c r="C5" s="19">
-        <v>0.46811606797228644</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.46811606797228644</v>
+      <c r="B5" s="39">
+        <v>0.80471675881350246</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1.0013873473917871</v>
+      </c>
+      <c r="D5" s="39">
+        <v>0.80471675881350246</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12">
-        <v>0.88024329921550515</v>
-      </c>
-      <c r="C6" s="19">
-        <v>0.42716732105660948</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.42716732105660948</v>
+      <c r="B6" s="38">
+        <v>0.75660088604365472</v>
+      </c>
+      <c r="C6" s="13">
+        <v>0.89</v>
+      </c>
+      <c r="D6" s="38">
+        <v>0.75660088604365472</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1288,8 +1347,8 @@
       <c r="C8" s="13">
         <v>0.8140954495005549</v>
       </c>
-      <c r="D8" s="5">
-        <v>0.76176470588235246</v>
+      <c r="D8" s="13">
+        <v>0.8140954495005549</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1302,8 +1361,8 @@
       <c r="C9" s="13">
         <v>1.0013873473917871</v>
       </c>
-      <c r="D9" s="5">
-        <v>0.73043478260869532</v>
+      <c r="D9" s="14">
+        <v>0.93661539708345787</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1358,8 +1417,8 @@
       <c r="C13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="5">
-        <v>0.62272727272727313</v>
+      <c r="D13" s="16">
+        <v>0.79806127394886706</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1372,8 +1431,8 @@
       <c r="C14" s="13">
         <v>1</v>
       </c>
-      <c r="D14" s="9">
-        <v>0.86996631266589408</v>
+      <c r="D14" s="44">
+        <v>0.75384615384615317</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1400,8 +1459,8 @@
       <c r="C16" s="13">
         <v>0.94556971627977604</v>
       </c>
-      <c r="D16" s="10">
-        <v>0.52857142857142891</v>
+      <c r="D16" s="11">
+        <v>0.89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1414,8 +1473,8 @@
       <c r="C17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="9">
-        <v>0.84920131314881475</v>
+      <c r="D17" s="41">
+        <v>0.76176470588235246</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1429,7 +1488,7 @@
         <v>42</v>
       </c>
       <c r="D18" s="5">
-        <v>0.66818181818181832</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1442,8 +1501,8 @@
       <c r="C19" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="31">
-        <v>0.5</v>
+      <c r="D19" s="45" t="s">
+        <v>168</v>
       </c>
       <c r="E19" t="s">
         <v>43</v>
@@ -1459,8 +1518,8 @@
       <c r="C20" s="13">
         <v>0.81470945228341618</v>
       </c>
-      <c r="D20" s="5">
-        <v>0.7447368421052627</v>
+      <c r="D20" s="44">
+        <v>0.76666666666666616</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1487,8 +1546,8 @@
       <c r="C22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="8">
-        <v>0.68736184357928687</v>
+      <c r="D22" s="41">
+        <v>0.62272727272727313</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1501,8 +1560,8 @@
       <c r="C23" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="10">
-        <v>0.50000000000000033</v>
+      <c r="D23" s="9">
+        <v>0.86962603256710036</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1515,8 +1574,8 @@
       <c r="C24" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="5">
-        <v>0.68333333333333313</v>
+      <c r="D24" s="9">
+        <v>0.85880942132039884</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1529,8 +1588,8 @@
       <c r="C25" s="13">
         <v>1</v>
       </c>
-      <c r="D25" s="8">
-        <v>0.78319614965094142</v>
+      <c r="D25" s="42">
+        <v>0.52857142857142891</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1571,8 +1630,8 @@
       <c r="C28" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="5">
-        <v>0.70526315789473681</v>
+      <c r="D28" s="41">
+        <v>0.76071428571428534</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1585,8 +1644,8 @@
       <c r="C29" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="10">
-        <v>0.46152597402597384</v>
+      <c r="D29" s="41">
+        <v>0.7447368421052627</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1599,8 +1658,8 @@
       <c r="C30" s="13">
         <v>0.88772568654225315</v>
       </c>
-      <c r="D30" s="5">
-        <v>0.66818181818181832</v>
+      <c r="D30" s="43">
+        <v>0.88772568654225315</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1613,8 +1672,8 @@
       <c r="C31" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="5">
-        <v>0.65000000000000024</v>
+      <c r="D31" s="41">
+        <v>0.78</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1627,8 +1686,8 @@
       <c r="C32" s="20">
         <v>0.70865588581341699</v>
       </c>
-      <c r="D32" s="7">
-        <v>0.70865588581341699</v>
+      <c r="D32" s="42">
+        <v>0.50000000000000033</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1641,8 +1700,8 @@
       <c r="C33" s="13">
         <v>0.9090980707958396</v>
       </c>
-      <c r="D33" s="9">
-        <v>0.81568198808221948</v>
+      <c r="D33" s="41">
+        <v>0.68333333333333313</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1772,12 +1831,18 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D12 D33:D35 D25:D26 D21:D22 D17 D14:D15" xr:uid="{8E57996F-529E-40AE-9A87-2868BAA73B75}">
-      <formula1>$M$2:$M$42</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C6" xr:uid="{E791450E-1821-4BAF-BE22-308C70C2B94E}">
+      <formula1>$P$3:$P$59</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2 B4:B42" xr:uid="{2094063A-1B54-4D04-B680-84EC71DE0C1C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C2 B7:C42" xr:uid="{8B6C5A4F-6A45-4774-823E-96EE9E70C3D8}">
       <formula1>$K$2:$K$42</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D6" xr:uid="{80199AEF-A48B-40F7-BCC4-5953C34445CF}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D34:D35 D26 D21 D23:D24 D9:D13 D15" xr:uid="{5661DA41-ECB0-4B36-9D0B-25AC62ADBCDB}">
+      <formula1>$N$2:$N$42</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1789,15 +1854,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4E5BEA-A0C4-45C8-A582-3EA5765DE126}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="6.88671875" style="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
@@ -1886,8 +1951,8 @@
       <c r="C5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="6">
-        <v>0.56226670149326563</v>
+      <c r="D5" s="40">
+        <v>0.75660088604365472</v>
       </c>
       <c r="E5" s="24" t="s">
         <v>48</v>
@@ -1904,7 +1969,7 @@
       <c r="C6" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="24"/>
       <c r="G6" s="36" t="s">
         <v>170</v>
@@ -1918,7 +1983,7 @@
       <c r="C7" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1931,8 +1996,8 @@
       <c r="C8" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="6">
-        <v>0.46811606797228644</v>
+      <c r="D8" s="39">
+        <v>0.80471675881350246</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>48</v>
@@ -1946,7 +2011,7 @@
       <c r="C9" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1959,8 +2024,8 @@
       <c r="C10" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.42716732105660948</v>
+      <c r="D10" s="40">
+        <v>0.75660088604365472</v>
       </c>
       <c r="E10" s="25" t="s">
         <v>49</v>
@@ -1993,8 +2058,8 @@
       <c r="C12" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="5">
-        <v>0.76176470588235246</v>
+      <c r="D12" s="13">
+        <v>0.8140954495005549</v>
       </c>
       <c r="E12" s="24" t="s">
         <v>48</v>
@@ -2010,8 +2075,8 @@
       <c r="C13" s="29">
         <v>5.9296671999999999</v>
       </c>
-      <c r="D13" s="5">
-        <v>0.73043478260869532</v>
+      <c r="D13" s="14">
+        <v>0.93661539708345787</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>49</v>
@@ -2111,8 +2176,8 @@
       <c r="C20" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="5">
-        <v>0.62272727272727313</v>
+      <c r="D20" s="16">
+        <v>0.79806127394886706</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>48</v>
@@ -2139,8 +2204,8 @@
       <c r="C22" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="9">
-        <v>0.86996631266589408</v>
+      <c r="D22" s="44">
+        <v>0.75384615384615317</v>
       </c>
       <c r="E22" s="25" t="s">
         <v>49</v>
@@ -2184,8 +2249,8 @@
       <c r="C25" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="10">
-        <v>0.52857142857142891</v>
+      <c r="D25" s="11">
+        <v>0.89</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>48</v>
@@ -2201,8 +2266,8 @@
       <c r="C26" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="9">
-        <v>0.84920131314881475</v>
+      <c r="D26" s="41">
+        <v>0.76176470588235246</v>
       </c>
       <c r="E26" s="24" t="s">
         <v>48</v>
@@ -2219,7 +2284,7 @@
         <v>101</v>
       </c>
       <c r="D27" s="5">
-        <v>0.66818181818181832</v>
+        <v>0.73</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>48</v>
@@ -2255,8 +2320,8 @@
       <c r="C29" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="5">
-        <v>0.7447368421052627</v>
+      <c r="D29" s="44">
+        <v>0.76666666666666616</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>48</v>
@@ -2289,8 +2354,8 @@
       <c r="C31" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="8">
-        <v>0.68736184357928687</v>
+      <c r="D31" s="41">
+        <v>0.62272727272727313</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>48</v>
@@ -2306,8 +2371,8 @@
       <c r="C32" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D32" s="10">
-        <v>0.50000000000000033</v>
+      <c r="D32" s="9">
+        <v>0.86962603256710036</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>48</v>
@@ -2323,8 +2388,8 @@
       <c r="C33" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="5">
-        <v>0.68333333333333313</v>
+      <c r="D33" s="9">
+        <v>0.85880942132039884</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>48</v>
@@ -2340,8 +2405,8 @@
       <c r="C34" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="8">
-        <v>0.78319614965094142</v>
+      <c r="D34" s="42">
+        <v>0.52857142857142891</v>
       </c>
       <c r="E34" s="25" t="s">
         <v>49</v>
@@ -2413,8 +2478,8 @@
       <c r="C39" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D39" s="5">
-        <v>0.70526315789473681</v>
+      <c r="D39" s="41">
+        <v>0.76071428571428534</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>48</v>
@@ -2430,8 +2495,8 @@
       <c r="C40" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="10">
-        <v>0.46152597402597384</v>
+      <c r="D40" s="41">
+        <v>0.7447368421052627</v>
       </c>
       <c r="E40" s="24" t="s">
         <v>48</v>
@@ -2447,8 +2512,8 @@
       <c r="C41" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="5">
-        <v>0.66818181818181832</v>
+      <c r="D41" s="43">
+        <v>0.88772568654225315</v>
       </c>
       <c r="E41" s="24" t="s">
         <v>48</v>
@@ -2464,8 +2529,8 @@
       <c r="C42" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="5">
-        <v>0.65000000000000024</v>
+      <c r="D42" s="41">
+        <v>0.78</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>48</v>
@@ -2492,8 +2557,8 @@
       <c r="C44" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="7">
-        <v>0.70865588581341699</v>
+      <c r="D44" s="42">
+        <v>0.50000000000000033</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>48</v>
@@ -2509,8 +2574,8 @@
       <c r="C45" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="9">
-        <v>0.81568198808221948</v>
+      <c r="D45" s="41">
+        <v>0.68333333333333313</v>
       </c>
       <c r="E45" s="24" t="s">
         <v>48</v>
@@ -2714,9 +2779,18 @@
       <c r="E58" s="24"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D30:D31 D34:D37 D45:D48 D14:D19 D22:D24 D26" xr:uid="{B204A10E-AA6F-4BA7-B9A1-EC0AFB8644E9}">
-      <formula1>$I$2:$I$42</formula1>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D35 D30 D32:D33" xr:uid="{FD7F0A6E-AB53-4426-9C6E-2A79CE010EB3}">
+      <formula1>$K$2:$K$42</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D36:D37 D5:D7 D9:D10 D14:D19 D46:D48 D23:D24" xr:uid="{F073254C-FD0E-40DB-85F3-6186902F5F15}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8" xr:uid="{E488430C-7D80-4439-AFB5-17E0B1723FC0}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D13 D20" xr:uid="{BD44717D-9011-4796-AE58-3D9838EF8D05}">
+      <formula1>$N$2:$N$42</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>